<commit_message>
upload maven ci script
</commit_message>
<xml_diff>
--- a/pe_sample/24SP-SWT301-FINAL-PE-Template.xlsx
+++ b/pe_sample/24SP-SWT301-FINAL-PE-Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Snake\FU\Teach\SP24\Evaluation\SWT301\PE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giao.lang\Desktop\_cloud.truong.lang\software-testing\pe_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="5" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>Function Code</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>a new receipt is successfully created</t>
-  </si>
-  <si>
-    <t>Create new receipt</t>
   </si>
   <si>
     <t>TC001</t>
@@ -342,6 +339,37 @@
   <si>
     <t>Test date
 (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Verify the Login UI conforming to the design</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Hoàng Ngọc Trinh</t>
+  </si>
+  <si>
+    <t>- An internet connection is available
+- The web app is available also</t>
+  </si>
+  <si>
+    <t>1. Open a certain browser, e.g. Chrome, CocCoc
+2. Navigate to the web app via url: https://passed-swp391.com
+3. Hit [Sign-in] button to open/reach the Login page/form</t>
+  </si>
+  <si>
+    <t>2. The homepage is shown with the [Sign-in] button located in the top-right
+3. The login page is displayed with the following elements:
+  - username/password labels and textboxes in case of logging in by SWP391 account
+    located in the center of the page
+  - [Login with Gmail] button in case of logging in by Gmail located under user/pass element
+  - [Login with Facebook] button in case of logging in by FB located under [Login with Gmail] 
+  - The logo of company is located in the top of the page
+  - The copyright statement with the current year is located in the bottom of the page</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1439,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1717,18 +1745,162 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="9" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="9" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1747,152 +1919,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2213,7 +2244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -2226,17 +2257,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="173" t="s">
+      <c r="B1" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="173" t="s">
+      <c r="C1" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="173" t="s">
-        <v>67</v>
+      <c r="D1" s="115" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2311,8 +2342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.199999999999999"/>
@@ -3092,56 +3123,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163" t="s">
+      <c r="D1" s="119"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
-      <c r="I1" s="164"/>
-      <c r="J1" s="164"/>
-      <c r="K1" s="164"/>
-      <c r="L1" s="165" t="s">
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="167"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="125"/>
     </row>
     <row r="2" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="168" t="s">
+      <c r="B2" s="127"/>
+      <c r="C2" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="169"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="142" t="s">
+      <c r="D2" s="129"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="171"/>
-      <c r="M2" s="171"/>
-      <c r="N2" s="171"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -3150,114 +3181,114 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140">
+      <c r="B3" s="127"/>
+      <c r="C3" s="142">
         <v>21</v>
       </c>
-      <c r="D3" s="141"/>
+      <c r="D3" s="143"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="142" t="s">
+      <c r="F3" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="145">
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="144">
         <v>-1</v>
       </c>
-      <c r="M3" s="146"/>
-      <c r="N3" s="146"/>
-      <c r="O3" s="146"/>
-      <c r="P3" s="146"/>
-      <c r="Q3" s="146"/>
-      <c r="R3" s="146"/>
-      <c r="S3" s="146"/>
-      <c r="T3" s="147"/>
+      <c r="M3" s="145"/>
+      <c r="N3" s="145"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="145"/>
+      <c r="Q3" s="145"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="146"/>
     </row>
     <row r="4" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="139"/>
-      <c r="C4" s="148" t="s">
+      <c r="B4" s="127"/>
+      <c r="C4" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="149"/>
-      <c r="G4" s="149"/>
-      <c r="H4" s="149"/>
-      <c r="I4" s="149"/>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="148"/>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="148"/>
-      <c r="S4" s="148"/>
-      <c r="T4" s="148"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="147"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="147"/>
+      <c r="O4" s="147"/>
+      <c r="P4" s="147"/>
+      <c r="Q4" s="147"/>
+      <c r="R4" s="147"/>
+      <c r="S4" s="147"/>
+      <c r="T4" s="147"/>
     </row>
     <row r="5" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A5" s="150" t="s">
+      <c r="A5" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="151"/>
-      <c r="C5" s="152" t="s">
+      <c r="B5" s="150"/>
+      <c r="C5" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="153"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="152" t="s">
+      <c r="D5" s="152"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="155"/>
-      <c r="L5" s="153" t="s">
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
+      <c r="J5" s="152"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="152" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="153"/>
-      <c r="N5" s="153"/>
-      <c r="O5" s="156" t="s">
+      <c r="M5" s="152"/>
+      <c r="N5" s="152"/>
+      <c r="O5" s="155" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="153"/>
-      <c r="Q5" s="153"/>
-      <c r="R5" s="153"/>
-      <c r="S5" s="153"/>
-      <c r="T5" s="157"/>
+      <c r="P5" s="152"/>
+      <c r="Q5" s="152"/>
+      <c r="R5" s="152"/>
+      <c r="S5" s="152"/>
+      <c r="T5" s="156"/>
     </row>
     <row r="6" spans="1:22" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="131">
+      <c r="A6" s="135">
         <f>COUNTIF(F40:HQ40,"P")</f>
         <v>0</v>
       </c>
-      <c r="B6" s="132"/>
-      <c r="C6" s="133">
+      <c r="B6" s="136"/>
+      <c r="C6" s="137">
         <f>COUNTIF(F40:HQ40,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="134"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="133">
+      <c r="D6" s="138"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="137">
         <f>SUM(O6,- A6,- C6)</f>
         <v>3</v>
       </c>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="135"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="138"/>
+      <c r="K6" s="139"/>
       <c r="L6" s="27">
         <f>COUNTIF(E39:HQ39,"N")</f>
         <v>1</v>
@@ -3270,32 +3301,32 @@
         <f>COUNTIF(E39:HQ39,"B")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="136">
+      <c r="O6" s="140">
         <f>COUNTA(E8:HT8)</f>
         <v>3</v>
       </c>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="134"/>
-      <c r="R6" s="134"/>
-      <c r="S6" s="134"/>
-      <c r="T6" s="137"/>
+      <c r="P6" s="138"/>
+      <c r="Q6" s="138"/>
+      <c r="R6" s="138"/>
+      <c r="S6" s="138"/>
+      <c r="T6" s="141"/>
       <c r="U6" s="6"/>
     </row>
     <row r="7" spans="1:22" ht="10.8" thickBot="1"/>
     <row r="8" spans="1:22" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A8" s="115"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
+      <c r="A8" s="165"/>
+      <c r="B8" s="166"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
       <c r="E8" s="39"/>
       <c r="F8" s="49" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50"/>
@@ -3538,10 +3569,10 @@
       <c r="A18" s="44"/>
       <c r="B18" s="41"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="117" t="s">
+      <c r="D18" s="163" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="118"/>
+      <c r="E18" s="164"/>
       <c r="F18" s="11" t="s">
         <v>16</v>
       </c>
@@ -3564,10 +3595,10 @@
       <c r="A19" s="44"/>
       <c r="B19" s="41"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="127" t="s">
+      <c r="D19" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="128"/>
+      <c r="E19" s="160"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11" t="s">
         <v>16</v>
@@ -3590,10 +3621,10 @@
       <c r="A20" s="44"/>
       <c r="B20" s="41"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="129" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="130"/>
+      <c r="D20" s="161" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="162"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11" t="s">
@@ -3638,8 +3669,8 @@
       <c r="A22" s="44"/>
       <c r="B22" s="41"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="118"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="164"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -3660,8 +3691,8 @@
       <c r="A23" s="44"/>
       <c r="B23" s="41"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="117"/>
-      <c r="E23" s="118"/>
+      <c r="D23" s="163"/>
+      <c r="E23" s="164"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3892,7 +3923,7 @@
       <c r="B33" s="73"/>
       <c r="C33" s="16"/>
       <c r="D33" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="11"/>
@@ -4031,11 +4062,11 @@
       <c r="A39" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="119" t="s">
+      <c r="B39" s="167" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="120"/>
-      <c r="D39" s="120"/>
+      <c r="C39" s="168"/>
+      <c r="D39" s="168"/>
       <c r="E39" s="64"/>
       <c r="F39" s="65" t="s">
         <v>23</v>
@@ -4057,11 +4088,11 @@
     </row>
     <row r="40" spans="1:20" ht="13.5" customHeight="1">
       <c r="A40" s="45"/>
-      <c r="B40" s="121" t="s">
+      <c r="B40" s="169" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="122"/>
-      <c r="D40" s="122"/>
+      <c r="C40" s="170"/>
+      <c r="D40" s="170"/>
       <c r="E40" s="19"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
@@ -4081,11 +4112,11 @@
     </row>
     <row r="41" spans="1:20" ht="13.5" customHeight="1">
       <c r="A41" s="45"/>
-      <c r="B41" s="123" t="s">
+      <c r="B41" s="171" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="124"/>
-      <c r="D41" s="124"/>
+      <c r="C41" s="172"/>
+      <c r="D41" s="172"/>
       <c r="E41" s="21"/>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -4105,11 +4136,11 @@
     </row>
     <row r="42" spans="1:20" ht="10.8" thickBot="1">
       <c r="A42" s="46"/>
-      <c r="B42" s="125" t="s">
+      <c r="B42" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="126"/>
-      <c r="D42" s="126"/>
+      <c r="C42" s="158"/>
+      <c r="D42" s="158"/>
       <c r="E42" s="36"/>
       <c r="F42" s="37"/>
       <c r="G42" s="37"/>
@@ -4146,14 +4177,16 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:K6"/>
@@ -4169,16 +4202,14 @@
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:T5"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:T1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVN983050:WWB983078 F65546:T65574 JB65546:JP65574 SX65546:TL65574 ACT65546:ADH65574 AMP65546:AND65574 AWL65546:AWZ65574 BGH65546:BGV65574 BQD65546:BQR65574 BZZ65546:CAN65574 CJV65546:CKJ65574 CTR65546:CUF65574 DDN65546:DEB65574 DNJ65546:DNX65574 DXF65546:DXT65574 EHB65546:EHP65574 EQX65546:ERL65574 FAT65546:FBH65574 FKP65546:FLD65574 FUL65546:FUZ65574 GEH65546:GEV65574 GOD65546:GOR65574 GXZ65546:GYN65574 HHV65546:HIJ65574 HRR65546:HSF65574 IBN65546:ICB65574 ILJ65546:ILX65574 IVF65546:IVT65574 JFB65546:JFP65574 JOX65546:JPL65574 JYT65546:JZH65574 KIP65546:KJD65574 KSL65546:KSZ65574 LCH65546:LCV65574 LMD65546:LMR65574 LVZ65546:LWN65574 MFV65546:MGJ65574 MPR65546:MQF65574 MZN65546:NAB65574 NJJ65546:NJX65574 NTF65546:NTT65574 ODB65546:ODP65574 OMX65546:ONL65574 OWT65546:OXH65574 PGP65546:PHD65574 PQL65546:PQZ65574 QAH65546:QAV65574 QKD65546:QKR65574 QTZ65546:QUN65574 RDV65546:REJ65574 RNR65546:ROF65574 RXN65546:RYB65574 SHJ65546:SHX65574 SRF65546:SRT65574 TBB65546:TBP65574 TKX65546:TLL65574 TUT65546:TVH65574 UEP65546:UFD65574 UOL65546:UOZ65574 UYH65546:UYV65574 VID65546:VIR65574 VRZ65546:VSN65574 WBV65546:WCJ65574 WLR65546:WMF65574 WVN65546:WWB65574 F131082:T131110 JB131082:JP131110 SX131082:TL131110 ACT131082:ADH131110 AMP131082:AND131110 AWL131082:AWZ131110 BGH131082:BGV131110 BQD131082:BQR131110 BZZ131082:CAN131110 CJV131082:CKJ131110 CTR131082:CUF131110 DDN131082:DEB131110 DNJ131082:DNX131110 DXF131082:DXT131110 EHB131082:EHP131110 EQX131082:ERL131110 FAT131082:FBH131110 FKP131082:FLD131110 FUL131082:FUZ131110 GEH131082:GEV131110 GOD131082:GOR131110 GXZ131082:GYN131110 HHV131082:HIJ131110 HRR131082:HSF131110 IBN131082:ICB131110 ILJ131082:ILX131110 IVF131082:IVT131110 JFB131082:JFP131110 JOX131082:JPL131110 JYT131082:JZH131110 KIP131082:KJD131110 KSL131082:KSZ131110 LCH131082:LCV131110 LMD131082:LMR131110 LVZ131082:LWN131110 MFV131082:MGJ131110 MPR131082:MQF131110 MZN131082:NAB131110 NJJ131082:NJX131110 NTF131082:NTT131110 ODB131082:ODP131110 OMX131082:ONL131110 OWT131082:OXH131110 PGP131082:PHD131110 PQL131082:PQZ131110 QAH131082:QAV131110 QKD131082:QKR131110 QTZ131082:QUN131110 RDV131082:REJ131110 RNR131082:ROF131110 RXN131082:RYB131110 SHJ131082:SHX131110 SRF131082:SRT131110 TBB131082:TBP131110 TKX131082:TLL131110 TUT131082:TVH131110 UEP131082:UFD131110 UOL131082:UOZ131110 UYH131082:UYV131110 VID131082:VIR131110 VRZ131082:VSN131110 WBV131082:WCJ131110 WLR131082:WMF131110 WVN131082:WWB131110 F196618:T196646 JB196618:JP196646 SX196618:TL196646 ACT196618:ADH196646 AMP196618:AND196646 AWL196618:AWZ196646 BGH196618:BGV196646 BQD196618:BQR196646 BZZ196618:CAN196646 CJV196618:CKJ196646 CTR196618:CUF196646 DDN196618:DEB196646 DNJ196618:DNX196646 DXF196618:DXT196646 EHB196618:EHP196646 EQX196618:ERL196646 FAT196618:FBH196646 FKP196618:FLD196646 FUL196618:FUZ196646 GEH196618:GEV196646 GOD196618:GOR196646 GXZ196618:GYN196646 HHV196618:HIJ196646 HRR196618:HSF196646 IBN196618:ICB196646 ILJ196618:ILX196646 IVF196618:IVT196646 JFB196618:JFP196646 JOX196618:JPL196646 JYT196618:JZH196646 KIP196618:KJD196646 KSL196618:KSZ196646 LCH196618:LCV196646 LMD196618:LMR196646 LVZ196618:LWN196646 MFV196618:MGJ196646 MPR196618:MQF196646 MZN196618:NAB196646 NJJ196618:NJX196646 NTF196618:NTT196646 ODB196618:ODP196646 OMX196618:ONL196646 OWT196618:OXH196646 PGP196618:PHD196646 PQL196618:PQZ196646 QAH196618:QAV196646 QKD196618:QKR196646 QTZ196618:QUN196646 RDV196618:REJ196646 RNR196618:ROF196646 RXN196618:RYB196646 SHJ196618:SHX196646 SRF196618:SRT196646 TBB196618:TBP196646 TKX196618:TLL196646 TUT196618:TVH196646 UEP196618:UFD196646 UOL196618:UOZ196646 UYH196618:UYV196646 VID196618:VIR196646 VRZ196618:VSN196646 WBV196618:WCJ196646 WLR196618:WMF196646 WVN196618:WWB196646 F262154:T262182 JB262154:JP262182 SX262154:TL262182 ACT262154:ADH262182 AMP262154:AND262182 AWL262154:AWZ262182 BGH262154:BGV262182 BQD262154:BQR262182 BZZ262154:CAN262182 CJV262154:CKJ262182 CTR262154:CUF262182 DDN262154:DEB262182 DNJ262154:DNX262182 DXF262154:DXT262182 EHB262154:EHP262182 EQX262154:ERL262182 FAT262154:FBH262182 FKP262154:FLD262182 FUL262154:FUZ262182 GEH262154:GEV262182 GOD262154:GOR262182 GXZ262154:GYN262182 HHV262154:HIJ262182 HRR262154:HSF262182 IBN262154:ICB262182 ILJ262154:ILX262182 IVF262154:IVT262182 JFB262154:JFP262182 JOX262154:JPL262182 JYT262154:JZH262182 KIP262154:KJD262182 KSL262154:KSZ262182 LCH262154:LCV262182 LMD262154:LMR262182 LVZ262154:LWN262182 MFV262154:MGJ262182 MPR262154:MQF262182 MZN262154:NAB262182 NJJ262154:NJX262182 NTF262154:NTT262182 ODB262154:ODP262182 OMX262154:ONL262182 OWT262154:OXH262182 PGP262154:PHD262182 PQL262154:PQZ262182 QAH262154:QAV262182 QKD262154:QKR262182 QTZ262154:QUN262182 RDV262154:REJ262182 RNR262154:ROF262182 RXN262154:RYB262182 SHJ262154:SHX262182 SRF262154:SRT262182 TBB262154:TBP262182 TKX262154:TLL262182 TUT262154:TVH262182 UEP262154:UFD262182 UOL262154:UOZ262182 UYH262154:UYV262182 VID262154:VIR262182 VRZ262154:VSN262182 WBV262154:WCJ262182 WLR262154:WMF262182 WVN262154:WWB262182 F327690:T327718 JB327690:JP327718 SX327690:TL327718 ACT327690:ADH327718 AMP327690:AND327718 AWL327690:AWZ327718 BGH327690:BGV327718 BQD327690:BQR327718 BZZ327690:CAN327718 CJV327690:CKJ327718 CTR327690:CUF327718 DDN327690:DEB327718 DNJ327690:DNX327718 DXF327690:DXT327718 EHB327690:EHP327718 EQX327690:ERL327718 FAT327690:FBH327718 FKP327690:FLD327718 FUL327690:FUZ327718 GEH327690:GEV327718 GOD327690:GOR327718 GXZ327690:GYN327718 HHV327690:HIJ327718 HRR327690:HSF327718 IBN327690:ICB327718 ILJ327690:ILX327718 IVF327690:IVT327718 JFB327690:JFP327718 JOX327690:JPL327718 JYT327690:JZH327718 KIP327690:KJD327718 KSL327690:KSZ327718 LCH327690:LCV327718 LMD327690:LMR327718 LVZ327690:LWN327718 MFV327690:MGJ327718 MPR327690:MQF327718 MZN327690:NAB327718 NJJ327690:NJX327718 NTF327690:NTT327718 ODB327690:ODP327718 OMX327690:ONL327718 OWT327690:OXH327718 PGP327690:PHD327718 PQL327690:PQZ327718 QAH327690:QAV327718 QKD327690:QKR327718 QTZ327690:QUN327718 RDV327690:REJ327718 RNR327690:ROF327718 RXN327690:RYB327718 SHJ327690:SHX327718 SRF327690:SRT327718 TBB327690:TBP327718 TKX327690:TLL327718 TUT327690:TVH327718 UEP327690:UFD327718 UOL327690:UOZ327718 UYH327690:UYV327718 VID327690:VIR327718 VRZ327690:VSN327718 WBV327690:WCJ327718 WLR327690:WMF327718 WVN327690:WWB327718 F393226:T393254 JB393226:JP393254 SX393226:TL393254 ACT393226:ADH393254 AMP393226:AND393254 AWL393226:AWZ393254 BGH393226:BGV393254 BQD393226:BQR393254 BZZ393226:CAN393254 CJV393226:CKJ393254 CTR393226:CUF393254 DDN393226:DEB393254 DNJ393226:DNX393254 DXF393226:DXT393254 EHB393226:EHP393254 EQX393226:ERL393254 FAT393226:FBH393254 FKP393226:FLD393254 FUL393226:FUZ393254 GEH393226:GEV393254 GOD393226:GOR393254 GXZ393226:GYN393254 HHV393226:HIJ393254 HRR393226:HSF393254 IBN393226:ICB393254 ILJ393226:ILX393254 IVF393226:IVT393254 JFB393226:JFP393254 JOX393226:JPL393254 JYT393226:JZH393254 KIP393226:KJD393254 KSL393226:KSZ393254 LCH393226:LCV393254 LMD393226:LMR393254 LVZ393226:LWN393254 MFV393226:MGJ393254 MPR393226:MQF393254 MZN393226:NAB393254 NJJ393226:NJX393254 NTF393226:NTT393254 ODB393226:ODP393254 OMX393226:ONL393254 OWT393226:OXH393254 PGP393226:PHD393254 PQL393226:PQZ393254 QAH393226:QAV393254 QKD393226:QKR393254 QTZ393226:QUN393254 RDV393226:REJ393254 RNR393226:ROF393254 RXN393226:RYB393254 SHJ393226:SHX393254 SRF393226:SRT393254 TBB393226:TBP393254 TKX393226:TLL393254 TUT393226:TVH393254 UEP393226:UFD393254 UOL393226:UOZ393254 UYH393226:UYV393254 VID393226:VIR393254 VRZ393226:VSN393254 WBV393226:WCJ393254 WLR393226:WMF393254 WVN393226:WWB393254 F458762:T458790 JB458762:JP458790 SX458762:TL458790 ACT458762:ADH458790 AMP458762:AND458790 AWL458762:AWZ458790 BGH458762:BGV458790 BQD458762:BQR458790 BZZ458762:CAN458790 CJV458762:CKJ458790 CTR458762:CUF458790 DDN458762:DEB458790 DNJ458762:DNX458790 DXF458762:DXT458790 EHB458762:EHP458790 EQX458762:ERL458790 FAT458762:FBH458790 FKP458762:FLD458790 FUL458762:FUZ458790 GEH458762:GEV458790 GOD458762:GOR458790 GXZ458762:GYN458790 HHV458762:HIJ458790 HRR458762:HSF458790 IBN458762:ICB458790 ILJ458762:ILX458790 IVF458762:IVT458790 JFB458762:JFP458790 JOX458762:JPL458790 JYT458762:JZH458790 KIP458762:KJD458790 KSL458762:KSZ458790 LCH458762:LCV458790 LMD458762:LMR458790 LVZ458762:LWN458790 MFV458762:MGJ458790 MPR458762:MQF458790 MZN458762:NAB458790 NJJ458762:NJX458790 NTF458762:NTT458790 ODB458762:ODP458790 OMX458762:ONL458790 OWT458762:OXH458790 PGP458762:PHD458790 PQL458762:PQZ458790 QAH458762:QAV458790 QKD458762:QKR458790 QTZ458762:QUN458790 RDV458762:REJ458790 RNR458762:ROF458790 RXN458762:RYB458790 SHJ458762:SHX458790 SRF458762:SRT458790 TBB458762:TBP458790 TKX458762:TLL458790 TUT458762:TVH458790 UEP458762:UFD458790 UOL458762:UOZ458790 UYH458762:UYV458790 VID458762:VIR458790 VRZ458762:VSN458790 WBV458762:WCJ458790 WLR458762:WMF458790 WVN458762:WWB458790 F524298:T524326 JB524298:JP524326 SX524298:TL524326 ACT524298:ADH524326 AMP524298:AND524326 AWL524298:AWZ524326 BGH524298:BGV524326 BQD524298:BQR524326 BZZ524298:CAN524326 CJV524298:CKJ524326 CTR524298:CUF524326 DDN524298:DEB524326 DNJ524298:DNX524326 DXF524298:DXT524326 EHB524298:EHP524326 EQX524298:ERL524326 FAT524298:FBH524326 FKP524298:FLD524326 FUL524298:FUZ524326 GEH524298:GEV524326 GOD524298:GOR524326 GXZ524298:GYN524326 HHV524298:HIJ524326 HRR524298:HSF524326 IBN524298:ICB524326 ILJ524298:ILX524326 IVF524298:IVT524326 JFB524298:JFP524326 JOX524298:JPL524326 JYT524298:JZH524326 KIP524298:KJD524326 KSL524298:KSZ524326 LCH524298:LCV524326 LMD524298:LMR524326 LVZ524298:LWN524326 MFV524298:MGJ524326 MPR524298:MQF524326 MZN524298:NAB524326 NJJ524298:NJX524326 NTF524298:NTT524326 ODB524298:ODP524326 OMX524298:ONL524326 OWT524298:OXH524326 PGP524298:PHD524326 PQL524298:PQZ524326 QAH524298:QAV524326 QKD524298:QKR524326 QTZ524298:QUN524326 RDV524298:REJ524326 RNR524298:ROF524326 RXN524298:RYB524326 SHJ524298:SHX524326 SRF524298:SRT524326 TBB524298:TBP524326 TKX524298:TLL524326 TUT524298:TVH524326 UEP524298:UFD524326 UOL524298:UOZ524326 UYH524298:UYV524326 VID524298:VIR524326 VRZ524298:VSN524326 WBV524298:WCJ524326 WLR524298:WMF524326 WVN524298:WWB524326 F589834:T589862 JB589834:JP589862 SX589834:TL589862 ACT589834:ADH589862 AMP589834:AND589862 AWL589834:AWZ589862 BGH589834:BGV589862 BQD589834:BQR589862 BZZ589834:CAN589862 CJV589834:CKJ589862 CTR589834:CUF589862 DDN589834:DEB589862 DNJ589834:DNX589862 DXF589834:DXT589862 EHB589834:EHP589862 EQX589834:ERL589862 FAT589834:FBH589862 FKP589834:FLD589862 FUL589834:FUZ589862 GEH589834:GEV589862 GOD589834:GOR589862 GXZ589834:GYN589862 HHV589834:HIJ589862 HRR589834:HSF589862 IBN589834:ICB589862 ILJ589834:ILX589862 IVF589834:IVT589862 JFB589834:JFP589862 JOX589834:JPL589862 JYT589834:JZH589862 KIP589834:KJD589862 KSL589834:KSZ589862 LCH589834:LCV589862 LMD589834:LMR589862 LVZ589834:LWN589862 MFV589834:MGJ589862 MPR589834:MQF589862 MZN589834:NAB589862 NJJ589834:NJX589862 NTF589834:NTT589862 ODB589834:ODP589862 OMX589834:ONL589862 OWT589834:OXH589862 PGP589834:PHD589862 PQL589834:PQZ589862 QAH589834:QAV589862 QKD589834:QKR589862 QTZ589834:QUN589862 RDV589834:REJ589862 RNR589834:ROF589862 RXN589834:RYB589862 SHJ589834:SHX589862 SRF589834:SRT589862 TBB589834:TBP589862 TKX589834:TLL589862 TUT589834:TVH589862 UEP589834:UFD589862 UOL589834:UOZ589862 UYH589834:UYV589862 VID589834:VIR589862 VRZ589834:VSN589862 WBV589834:WCJ589862 WLR589834:WMF589862 WVN589834:WWB589862 F655370:T655398 JB655370:JP655398 SX655370:TL655398 ACT655370:ADH655398 AMP655370:AND655398 AWL655370:AWZ655398 BGH655370:BGV655398 BQD655370:BQR655398 BZZ655370:CAN655398 CJV655370:CKJ655398 CTR655370:CUF655398 DDN655370:DEB655398 DNJ655370:DNX655398 DXF655370:DXT655398 EHB655370:EHP655398 EQX655370:ERL655398 FAT655370:FBH655398 FKP655370:FLD655398 FUL655370:FUZ655398 GEH655370:GEV655398 GOD655370:GOR655398 GXZ655370:GYN655398 HHV655370:HIJ655398 HRR655370:HSF655398 IBN655370:ICB655398 ILJ655370:ILX655398 IVF655370:IVT655398 JFB655370:JFP655398 JOX655370:JPL655398 JYT655370:JZH655398 KIP655370:KJD655398 KSL655370:KSZ655398 LCH655370:LCV655398 LMD655370:LMR655398 LVZ655370:LWN655398 MFV655370:MGJ655398 MPR655370:MQF655398 MZN655370:NAB655398 NJJ655370:NJX655398 NTF655370:NTT655398 ODB655370:ODP655398 OMX655370:ONL655398 OWT655370:OXH655398 PGP655370:PHD655398 PQL655370:PQZ655398 QAH655370:QAV655398 QKD655370:QKR655398 QTZ655370:QUN655398 RDV655370:REJ655398 RNR655370:ROF655398 RXN655370:RYB655398 SHJ655370:SHX655398 SRF655370:SRT655398 TBB655370:TBP655398 TKX655370:TLL655398 TUT655370:TVH655398 UEP655370:UFD655398 UOL655370:UOZ655398 UYH655370:UYV655398 VID655370:VIR655398 VRZ655370:VSN655398 WBV655370:WCJ655398 WLR655370:WMF655398 WVN655370:WWB655398 F720906:T720934 JB720906:JP720934 SX720906:TL720934 ACT720906:ADH720934 AMP720906:AND720934 AWL720906:AWZ720934 BGH720906:BGV720934 BQD720906:BQR720934 BZZ720906:CAN720934 CJV720906:CKJ720934 CTR720906:CUF720934 DDN720906:DEB720934 DNJ720906:DNX720934 DXF720906:DXT720934 EHB720906:EHP720934 EQX720906:ERL720934 FAT720906:FBH720934 FKP720906:FLD720934 FUL720906:FUZ720934 GEH720906:GEV720934 GOD720906:GOR720934 GXZ720906:GYN720934 HHV720906:HIJ720934 HRR720906:HSF720934 IBN720906:ICB720934 ILJ720906:ILX720934 IVF720906:IVT720934 JFB720906:JFP720934 JOX720906:JPL720934 JYT720906:JZH720934 KIP720906:KJD720934 KSL720906:KSZ720934 LCH720906:LCV720934 LMD720906:LMR720934 LVZ720906:LWN720934 MFV720906:MGJ720934 MPR720906:MQF720934 MZN720906:NAB720934 NJJ720906:NJX720934 NTF720906:NTT720934 ODB720906:ODP720934 OMX720906:ONL720934 OWT720906:OXH720934 PGP720906:PHD720934 PQL720906:PQZ720934 QAH720906:QAV720934 QKD720906:QKR720934 QTZ720906:QUN720934 RDV720906:REJ720934 RNR720906:ROF720934 RXN720906:RYB720934 SHJ720906:SHX720934 SRF720906:SRT720934 TBB720906:TBP720934 TKX720906:TLL720934 TUT720906:TVH720934 UEP720906:UFD720934 UOL720906:UOZ720934 UYH720906:UYV720934 VID720906:VIR720934 VRZ720906:VSN720934 WBV720906:WCJ720934 WLR720906:WMF720934 WVN720906:WWB720934 F786442:T786470 JB786442:JP786470 SX786442:TL786470 ACT786442:ADH786470 AMP786442:AND786470 AWL786442:AWZ786470 BGH786442:BGV786470 BQD786442:BQR786470 BZZ786442:CAN786470 CJV786442:CKJ786470 CTR786442:CUF786470 DDN786442:DEB786470 DNJ786442:DNX786470 DXF786442:DXT786470 EHB786442:EHP786470 EQX786442:ERL786470 FAT786442:FBH786470 FKP786442:FLD786470 FUL786442:FUZ786470 GEH786442:GEV786470 GOD786442:GOR786470 GXZ786442:GYN786470 HHV786442:HIJ786470 HRR786442:HSF786470 IBN786442:ICB786470 ILJ786442:ILX786470 IVF786442:IVT786470 JFB786442:JFP786470 JOX786442:JPL786470 JYT786442:JZH786470 KIP786442:KJD786470 KSL786442:KSZ786470 LCH786442:LCV786470 LMD786442:LMR786470 LVZ786442:LWN786470 MFV786442:MGJ786470 MPR786442:MQF786470 MZN786442:NAB786470 NJJ786442:NJX786470 NTF786442:NTT786470 ODB786442:ODP786470 OMX786442:ONL786470 OWT786442:OXH786470 PGP786442:PHD786470 PQL786442:PQZ786470 QAH786442:QAV786470 QKD786442:QKR786470 QTZ786442:QUN786470 RDV786442:REJ786470 RNR786442:ROF786470 RXN786442:RYB786470 SHJ786442:SHX786470 SRF786442:SRT786470 TBB786442:TBP786470 TKX786442:TLL786470 TUT786442:TVH786470 UEP786442:UFD786470 UOL786442:UOZ786470 UYH786442:UYV786470 VID786442:VIR786470 VRZ786442:VSN786470 WBV786442:WCJ786470 WLR786442:WMF786470 WVN786442:WWB786470 F851978:T852006 JB851978:JP852006 SX851978:TL852006 ACT851978:ADH852006 AMP851978:AND852006 AWL851978:AWZ852006 BGH851978:BGV852006 BQD851978:BQR852006 BZZ851978:CAN852006 CJV851978:CKJ852006 CTR851978:CUF852006 DDN851978:DEB852006 DNJ851978:DNX852006 DXF851978:DXT852006 EHB851978:EHP852006 EQX851978:ERL852006 FAT851978:FBH852006 FKP851978:FLD852006 FUL851978:FUZ852006 GEH851978:GEV852006 GOD851978:GOR852006 GXZ851978:GYN852006 HHV851978:HIJ852006 HRR851978:HSF852006 IBN851978:ICB852006 ILJ851978:ILX852006 IVF851978:IVT852006 JFB851978:JFP852006 JOX851978:JPL852006 JYT851978:JZH852006 KIP851978:KJD852006 KSL851978:KSZ852006 LCH851978:LCV852006 LMD851978:LMR852006 LVZ851978:LWN852006 MFV851978:MGJ852006 MPR851978:MQF852006 MZN851978:NAB852006 NJJ851978:NJX852006 NTF851978:NTT852006 ODB851978:ODP852006 OMX851978:ONL852006 OWT851978:OXH852006 PGP851978:PHD852006 PQL851978:PQZ852006 QAH851978:QAV852006 QKD851978:QKR852006 QTZ851978:QUN852006 RDV851978:REJ852006 RNR851978:ROF852006 RXN851978:RYB852006 SHJ851978:SHX852006 SRF851978:SRT852006 TBB851978:TBP852006 TKX851978:TLL852006 TUT851978:TVH852006 UEP851978:UFD852006 UOL851978:UOZ852006 UYH851978:UYV852006 VID851978:VIR852006 VRZ851978:VSN852006 WBV851978:WCJ852006 WLR851978:WMF852006 WVN851978:WWB852006 F917514:T917542 JB917514:JP917542 SX917514:TL917542 ACT917514:ADH917542 AMP917514:AND917542 AWL917514:AWZ917542 BGH917514:BGV917542 BQD917514:BQR917542 BZZ917514:CAN917542 CJV917514:CKJ917542 CTR917514:CUF917542 DDN917514:DEB917542 DNJ917514:DNX917542 DXF917514:DXT917542 EHB917514:EHP917542 EQX917514:ERL917542 FAT917514:FBH917542 FKP917514:FLD917542 FUL917514:FUZ917542 GEH917514:GEV917542 GOD917514:GOR917542 GXZ917514:GYN917542 HHV917514:HIJ917542 HRR917514:HSF917542 IBN917514:ICB917542 ILJ917514:ILX917542 IVF917514:IVT917542 JFB917514:JFP917542 JOX917514:JPL917542 JYT917514:JZH917542 KIP917514:KJD917542 KSL917514:KSZ917542 LCH917514:LCV917542 LMD917514:LMR917542 LVZ917514:LWN917542 MFV917514:MGJ917542 MPR917514:MQF917542 MZN917514:NAB917542 NJJ917514:NJX917542 NTF917514:NTT917542 ODB917514:ODP917542 OMX917514:ONL917542 OWT917514:OXH917542 PGP917514:PHD917542 PQL917514:PQZ917542 QAH917514:QAV917542 QKD917514:QKR917542 QTZ917514:QUN917542 RDV917514:REJ917542 RNR917514:ROF917542 RXN917514:RYB917542 SHJ917514:SHX917542 SRF917514:SRT917542 TBB917514:TBP917542 TKX917514:TLL917542 TUT917514:TVH917542 UEP917514:UFD917542 UOL917514:UOZ917542 UYH917514:UYV917542 VID917514:VIR917542 VRZ917514:VSN917542 WBV917514:WCJ917542 WLR917514:WMF917542 WVN917514:WWB917542 F983050:T983078 JB983050:JP983078 SX983050:TL983078 ACT983050:ADH983078 AMP983050:AND983078 AWL983050:AWZ983078 BGH983050:BGV983078 BQD983050:BQR983078 BZZ983050:CAN983078 CJV983050:CKJ983078 CTR983050:CUF983078 DDN983050:DEB983078 DNJ983050:DNX983078 DXF983050:DXT983078 EHB983050:EHP983078 EQX983050:ERL983078 FAT983050:FBH983078 FKP983050:FLD983078 FUL983050:FUZ983078 GEH983050:GEV983078 GOD983050:GOR983078 GXZ983050:GYN983078 HHV983050:HIJ983078 HRR983050:HSF983078 IBN983050:ICB983078 ILJ983050:ILX983078 IVF983050:IVT983078 JFB983050:JFP983078 JOX983050:JPL983078 JYT983050:JZH983078 KIP983050:KJD983078 KSL983050:KSZ983078 LCH983050:LCV983078 LMD983050:LMR983078 LVZ983050:LWN983078 MFV983050:MGJ983078 MPR983050:MQF983078 MZN983050:NAB983078 NJJ983050:NJX983078 NTF983050:NTT983078 ODB983050:ODP983078 OMX983050:ONL983078 OWT983050:OXH983078 PGP983050:PHD983078 PQL983050:PQZ983078 QAH983050:QAV983078 QKD983050:QKR983078 QTZ983050:QUN983078 RDV983050:REJ983078 RNR983050:ROF983078 RXN983050:RYB983078 SHJ983050:SHX983078 SRF983050:SRT983078 TBB983050:TBP983078 TKX983050:TLL983078 TUT983050:TVH983078 UEP983050:UFD983078 UOL983050:UOZ983078 UYH983050:UYV983078 VID983050:VIR983078 VRZ983050:VSN983078 WBV983050:WCJ983078 WLR983050:WMF983078 JB9:JP38 WVN9:WWB38 WLR9:WMF38 WBV9:WCJ38 VRZ9:VSN38 VID9:VIR38 UYH9:UYV38 UOL9:UOZ38 UEP9:UFD38 TUT9:TVH38 TKX9:TLL38 TBB9:TBP38 SRF9:SRT38 SHJ9:SHX38 RXN9:RYB38 RNR9:ROF38 RDV9:REJ38 QTZ9:QUN38 QKD9:QKR38 QAH9:QAV38 PQL9:PQZ38 PGP9:PHD38 OWT9:OXH38 OMX9:ONL38 ODB9:ODP38 NTF9:NTT38 NJJ9:NJX38 MZN9:NAB38 MPR9:MQF38 MFV9:MGJ38 LVZ9:LWN38 LMD9:LMR38 LCH9:LCV38 KSL9:KSZ38 KIP9:KJD38 JYT9:JZH38 JOX9:JPL38 JFB9:JFP38 IVF9:IVT38 ILJ9:ILX38 IBN9:ICB38 HRR9:HSF38 HHV9:HIJ38 GXZ9:GYN38 GOD9:GOR38 GEH9:GEV38 FUL9:FUZ38 FKP9:FLD38 FAT9:FBH38 EQX9:ERL38 EHB9:EHP38 DXF9:DXT38 DNJ9:DNX38 DDN9:DEB38 CTR9:CUF38 CJV9:CKJ38 BZZ9:CAN38 BQD9:BQR38 BGH9:BGV38 AWL9:AWZ38 AMP9:AND38 ACT9:ADH38 SX9:TL38 H33 F9:T31 F34:T38 F32:G33 I32:T33">
@@ -4201,17 +4232,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.199999999999999"/>
   <cols>
     <col min="1" max="1" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="24" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="40" style="24" customWidth="1"/>
     <col min="6" max="6" width="11.109375" style="24" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" style="24" customWidth="1"/>
     <col min="8" max="8" width="14.109375" style="24" customWidth="1"/>
@@ -4220,17 +4251,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.399999999999999">
-      <c r="A1" s="172" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
+      <c r="A1" s="173" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
     </row>
     <row r="2" spans="1:9" ht="13.8">
       <c r="A2" s="92"/>
@@ -4254,7 +4285,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="100"/>
       <c r="D3" s="94" t="str">
@@ -4275,7 +4306,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C4" s="101"/>
       <c r="D4" s="102" t="str">
@@ -4284,7 +4315,7 @@
       </c>
       <c r="E4" s="103" t="str">
         <f>"Number of cases: "&amp;(COUNTA($A$6:$A$942))</f>
-        <v>Number of cases: 2</v>
+        <v>Number of cases: 3</v>
       </c>
       <c r="F4" s="92"/>
       <c r="G4" s="104"/>
@@ -4314,7 +4345,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="114" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="114" t="s">
         <v>35</v>
@@ -4322,40 +4353,56 @@
     </row>
     <row r="6" spans="1:9" ht="61.2">
       <c r="A6" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="C6" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="D6" s="112" t="s">
         <v>59</v>
-      </c>
-      <c r="D6" s="112" t="s">
-        <v>60</v>
       </c>
       <c r="E6" s="112" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="111" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="112" t="s">
         <v>45</v>
       </c>
       <c r="H6" s="113"/>
       <c r="I6" s="112" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="84"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="86"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="109.2" customHeight="1">
+      <c r="A7" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="174" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="86">
+        <v>45483</v>
+      </c>
       <c r="I7" s="84"/>
     </row>
     <row r="8" spans="1:9">

</xml_diff>